<commit_message>
Add '-' and download
</commit_message>
<xml_diff>
--- a/grupowsp.xlsx
+++ b/grupowsp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D5D1A6-8C21-4837-9EB4-5D51F69128E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9116F8-E3E8-4A09-A630-1813B82629FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="383">
   <si>
     <t>N°</t>
   </si>
@@ -728,9 +728,6 @@
     <t>https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>&lt;span role='presentation' style='padding-right: 0.1px'&gt;&lt;/span&gt;</t>
   </si>
   <si>
@@ -774,13 +771,412 @@
   </si>
   <si>
     <t>SECCION</t>
+  </si>
+  <si>
+    <t>BACKUP</t>
+  </si>
+  <si>
+    <t>TAMAÑO</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69101/backup/course/II-M-ACULTURA%20AMBIENTAL%20-%202767.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>286.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69107/backup/course/II-T-BCULTURA%20AMBIENTAL%20-%202773.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>271.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69097/backup/course/II-M-AAN%C3%81LISIS%20MATEM%C3%81TICO%20-%202763.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>49.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69103/backup/course/II-T-BAN%C3%81LISIS%20MATEM%C3%81TICO%20-%202769.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>90MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69098/backup/course/II-M-AF%C3%8DSICA%20-%202764.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>1MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69104/backup/course/II-T-BF%C3%8DSICA%20-%202770.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>12.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69099/backup/course/II-M-AQU%C3%8DMICA%20GENERAL%20-%202765.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>346.1MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69105/backup/course/II-T-BQU%C3%8DMICA%20GENERAL%20-%202771.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>190MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69100/backup/course/II-M-ABOT%C3%81NICA%20GENERAL%20-%202766.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>582.3MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69106/backup/course/II-T-BBOT%C3%81NICA%20GENERAL%20-%202772.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>603.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69102/backup/course/II-M-AINFORM%C3%81TICA%20-%202768.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>740.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69108/backup/course/II-T-BINFORM%C3%81TICA%20-%202774.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>502.3MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69110/backup/course/IV-M-ABIOQU%C3%8DMICA%20GENERAL%20-%202776.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>137.1MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69116/backup/course/IV-T-BBIOQU%C3%8DMICA%20GENERAL%20-%202782.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>115.7MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69111/backup/course/IV-M-AESTAD%C3%8DSTICA%20GENERAL%20-%202777.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>22.7MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69117/backup/course/IV-T-BESTAD%C3%8DSTICA%20GENERAL%20-%202783.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>35.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69112/backup/course/IV-M-AF%C3%8DSICA%20II%20-%202778.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>1005.2KB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69118/backup/course/IV-T-BF%C3%8DSICA%20II%20-%202784.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>828.9KB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69113/backup/course/IV-M-AAGROECOLOG%C3%8DA%20-%202779.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>33.4MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69119/backup/course/IV-T-BAGROECOLOG%C3%8DA%20-%202785.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>24.1MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69114/backup/course/IV-M-AMICROECONOM%C3%8DA%20-%202780.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>73.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69120/backup/course/IV-T-BMICROECONOM%C3%8DA%20-%202786.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>95.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69109/backup/course/IV-M-ALIDERAZGO%20Y%20TRABAJO%20EN%20EQUIPO%20-%202775.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>13.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69115/backup/course/IV-T-BLIDERAZGO%20Y%20TRABAJO%20EN%20EQUIPO%20-%202781.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>14.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69122/backup/course/V-T-AMECANIZACI%C3%93N%20AGR%C3%8DCOLA%20-%202788.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>827.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69123/backup/course/V-T-AFISIOLOG%C3%8DA%20VEGETAL%20-%202789.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>930.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69124/backup/course/V-T-AGEN%C3%89TICA%20VEGETAL%20-%202790.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>226.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69125/backup/course/V-T-AMETEOROLOG%C3%8DA%20-%202791.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>41.3MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69126/backup/course/V-T-AMICROBIOLOG%C3%8DA%20-%202792.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>297.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69121/backup/course/V-T-ACONSTITUCI%C3%93N%20Y%20DERECHOS%20HUMANOS%20-%202787.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>41.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69127/backup/course/V-T-AEDAFOLOGIA%20-%202793.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>3.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69129/backup/course/VI-T-AAGROTECN%C3%8DA%20-%202795.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>112.3MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69130/backup/course/VI-T-AFERTILIDAD%20DEL%20SUELO%20-%202796.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>6.4MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69131/backup/course/VI-T-APROPAGACI%C3%93N%20DE%20PLANTAS%20-%202797.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>482MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69132/backup/course/VI-T-AENTOMOLOG%C3%8DA%20GENERAL%20-%202798.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>217.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69133/backup/course/VI-T-ATOPOGRAF%C3%8DA%20-%202799.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>65.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69128/backup/course/VI-T-APENSAMIENTO%20POL%C3%8DTICO%20CONTEMPOR%C3%81NEO%20-%202794.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>61.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69134/backup/course/VIII-M-ARAICES%20Y%20TUB%C3%89RCULOS%20-%202800.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>94.4MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69140/backup/course/VIII-T-BRAICES%20Y%20TUB%C3%89RCULOS%20-%202806.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>93.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69135/backup/course/VIII-M-AOLERICULTURA%20-%202801.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>252.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69141/backup/course/VIII-T-BOLERICULTURA%20-%202807.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>145.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69136/backup/course/VIII-M-AFRUTICULTURA%20-%202802.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>910.9MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69142/backup/course/VIII-T-BFRUTICULTURA%20-%202808.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>496.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69139/backup/course/VIII-M-AENTOMOLOG%C3%8DA%20AGR%C3%8DCOLA%20-%202805.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>75.7MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69145/backup/course/VIII-T-BENTOMOLOG%C3%8DA%20AGR%C3%8DCOLA%20-%202811.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>55.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69137/backup/course/VIII-M-AMETODOLOG%C3%8DA%20DE%20INVESTIGACI%C3%93N%20CIENT%C3%8DFICA%20-%202803.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>252.4MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69143/backup/course/VIII-T-BMETODOLOG%C3%8DA%20DE%20INVESTIGACI%C3%93N%20CIENT%C3%8DFICA%20-%202809.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>156.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69138/backup/course/VIII-M-APRODUCCI%C3%93N%20DE%20SEMILLAS%20-%202804.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>286MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69144/backup/course/VIII-T-BPRODUCCI%C3%93N%20DE%20SEMILLAS%20-%202810.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>160.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69146/backup/course/X-M-AFORMULACI%C3%93N%20Y%20EVALUACI%C3%93N%20DE%20PROYECTOS%20AGR%C3%8DCOLAS%20-%202812.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>68MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69159/backup/course/X-T-BFORMULACI%C3%93N%20Y%20EVALUACI%C3%93N%20DE%20PROYECTOS%20AGR%C3%8DCOLAS%20-%202819.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>65.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69149/backup/course/X-M-AEXTENSI%C3%93N%20AGRARIA%20-%202815.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>158.4MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69156/backup/course/X-T-BEXTENSI%C3%93N%20AGRARIA%20-%202822.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>298.1MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69147/backup/course/X-M-AMANEJO%20INTEGRADO%20DE%20PLAGAS%20Y%20ENFERMEDADES%20-%202813.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>138.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69158/backup/course/X-T-BMANEJO%20INTEGRADO%20DE%20PLAGAS%20Y%20ENFERMEDADES%20-%202820.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>147.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69148/backup/course/X-M-ASEMINARIO%20DE%20TESIS%20II%20-%202814.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>98.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69157/backup/course/X-T-BSEMINARIO%20DE%20TESIS%20II%20-%202821.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>341.8MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69150/backup/course/X-M-ANUTRICI%C3%93N%20Y%20ALIMENTACI%C3%93N%20ANIMAL%20-%202816.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>194.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69155/backup/course/X-T-BNUTRICI%C3%93N%20Y%20ALIMENTACI%C3%93N%20ANIMAL%20-%202823.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>222.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69151/backup/course/X-M-ACONTROL%20BIOL%C3%93GICO%20DE%20PLAGAS%20Y%20ENFERMEDADES%20-%202817.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69154/backup/course/X-T-BCONTROL%20BIOL%C3%93GICO%20DE%20PLAGAS%20Y%20ENFERMEDADES%20-%202824.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>174.5MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69152/backup/course/X-M-AAGRICULTURA%20ORG%C3%81NICA%20Y%20CERTIFICACIONES%20-%202818.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>702.2KB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/69153/backup/course/X-T-BAGRICULTURA%20ORG%C3%81NICA%20Y%20CERTIFICACIONES%20-%202825.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>1.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/72047/backup/course/III-M-AMATEM%C3%81TICA%20II%20-%202850.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>739.2MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/71640/backup/course/I-M-AMATEM%C3%81TICA%20B%C3%81SICA%20-%202849.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>328.6MB</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/pluginfile.php/73252/backup/course/V-T-BEDAFOLOGIA%20-%202756.mbz?forcedownload=1</t>
+  </si>
+  <si>
+    <t>484.4MB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,6 +1201,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -836,7 +1240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -881,12 +1285,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -912,6 +1331,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1216,11 +1639,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AB67"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,14 +1661,16 @@
     <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.85546875" customWidth="1"/>
+    <col min="23" max="23" width="27.42578125" customWidth="1"/>
     <col min="24" max="24" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.5703125" customWidth="1"/>
-    <col min="27" max="27" width="140.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" customWidth="1"/>
+    <col min="28" max="28" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1285,7 +1710,7 @@
         <v>8</v>
       </c>
       <c r="U1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V1" s="5" t="s">
         <v>2</v>
@@ -1302,8 +1727,14 @@
       <c r="Z1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA1" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1361,17 +1792,20 @@
         <v>AG_II-M-A CULTURA AMBIENT</v>
       </c>
       <c r="Z2" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S2,"' target='_blank'&gt;&lt;img src='",AA2,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S2,"' target='_blank'&gt;&lt;img src='",AC2,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LWJSKSqib1fH6uocU35PYb' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC2" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1429,17 +1863,20 @@
         <v>AG_II-T-B CULTURA AMBIENT</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z64" si="9">CONCATENATE("&lt;p&gt;&lt;a href='",S3,"' target='_blank'&gt;&lt;img src='",AA3,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S3,"' target='_blank'&gt;&lt;img src='",AC3,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JWMiL8dNxPQ642NljMskFw' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AA3" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC3" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1497,17 +1934,20 @@
         <v>AG_II-M-A ANÁLISIS MATEMÁ</v>
       </c>
       <c r="Z4" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S4,"' target='_blank'&gt;&lt;img src='",AC4,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BVsq7GvIbpzLPDxWuh9RXx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AA4" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1565,17 +2005,20 @@
         <v>AG_II-T-B ANÁLISIS MATEMÁ</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S5,"' target='_blank'&gt;&lt;img src='",AC5,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CnT9oBWGpph5yKj8Nfz5c5' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AA5" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AC5" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1633,17 +2076,20 @@
         <v>AG_II-M-A FÍSICA - 2764</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S6,"' target='_blank'&gt;&lt;img src='",AC6,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/HsXEKyk5ZOLFDK4Y4GWwLA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AA6" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC6" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1701,17 +2147,20 @@
         <v>AG_II-T-B FÍSICA - 2770</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S7,"' target='_blank'&gt;&lt;img src='",AC7,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CfAVpDRlBdX4E1zem4qrEn' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AA7" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC7" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1769,17 +2218,20 @@
         <v>AG_II-M-A QUÍMICA GENERAL</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S8,"' target='_blank'&gt;&lt;img src='",AC8,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IOUAT3LwFHCA0Fr2PrS7Ui' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AA8" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC8" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1837,17 +2289,20 @@
         <v>AG_II-T-B QUÍMICA GENERAL</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S9,"' target='_blank'&gt;&lt;img src='",AC9,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KtuxNltmEqWDFhw2RVnVho' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA9" s="8" t="s">
+      <c r="AA9" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>267</v>
+      </c>
+      <c r="AC9" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1905,17 +2360,20 @@
         <v>AG_II-M-A BOTÁNICA GENERA</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S10,"' target='_blank'&gt;&lt;img src='",AC10,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KPsHkXMLMet6faBGdSZQex' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA10" s="8" t="s">
+      <c r="AA10" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC10" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1973,17 +2431,20 @@
         <v>AG_II-T-B BOTÁNICA GENERA</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S11,"' target='_blank'&gt;&lt;img src='",AC11,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J0LEUV90FrjJX778c2ietI' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA11" s="8" t="s">
+      <c r="AA11" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC11" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2041,17 +2502,20 @@
         <v>AG_II-M-A INFORMÁTICA - 2</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S12,"' target='_blank'&gt;&lt;img src='",AC12,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LiqhSZJoUyFDPPWBahSaXq' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA12" s="8" t="s">
+      <c r="AA12" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>273</v>
+      </c>
+      <c r="AC12" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2109,17 +2573,20 @@
         <v>AG_II-T-B INFORMÁTICA - 2</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S13,"' target='_blank'&gt;&lt;img src='",AC13,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CaWfkGJVannHNmr4bBlYaA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA13" s="8" t="s">
+      <c r="AA13" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC13" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2177,17 +2644,20 @@
         <v>AG_IV-M-A BIOQUÍMICA GENE</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S14,"' target='_blank'&gt;&lt;img src='",AC14,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FF4MoK2k3Bp2JRfHWFtn2e' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA14" s="8" t="s">
+      <c r="AA14" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC14" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2245,17 +2715,20 @@
         <v>AG_IV-T-B BIOQUÍMICA GENE</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S15,"' target='_blank'&gt;&lt;img src='",AC15,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Ikat0W4Vkjc9DOM8k1zrwa' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA15" s="8" t="s">
+      <c r="AA15" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>279</v>
+      </c>
+      <c r="AC15" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2313,17 +2786,20 @@
         <v>AG_IV-M-A ESTADÍSTICA GEN</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S16,"' target='_blank'&gt;&lt;img src='",AC16,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J7kjcXw4SeP6Lm2yB4s0Hd' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA16" s="8" t="s">
+      <c r="AA16" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>281</v>
+      </c>
+      <c r="AC16" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB16" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2381,17 +2857,20 @@
         <v>AG_IV-T-B ESTADÍSTICA GEN</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S17,"' target='_blank'&gt;&lt;img src='",AC17,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Jv66x356fa84eqiAZibbtB' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA17" s="8" t="s">
+      <c r="AA17" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC17" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2449,17 +2928,20 @@
         <v>AG_IV-M-A FÍSICA II - 277</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S18,"' target='_blank'&gt;&lt;img src='",AC18,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DbzaveELGys0X6N50SABYq' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA18" s="8" t="s">
+      <c r="AA18" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>285</v>
+      </c>
+      <c r="AC18" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2517,17 +2999,20 @@
         <v>AG_IV-T-B FÍSICA II - 278</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S19,"' target='_blank'&gt;&lt;img src='",AC19,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BYJKAz8Qvkg6rgwCjQQYfm' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA19" s="8" t="s">
+      <c r="AA19" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC19" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2585,17 +3070,20 @@
         <v xml:space="preserve">AG_IV-M-A AGROECOLOGÍA - </v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S20,"' target='_blank'&gt;&lt;img src='",AC20,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LrEwv8Dfv1Z1gYTj2DuKfo' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA20" s="8" t="s">
+      <c r="AA20" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC20" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2653,17 +3141,20 @@
         <v xml:space="preserve">AG_IV-T-B AGROECOLOGÍA - </v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S21,"' target='_blank'&gt;&lt;img src='",AC21,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BojTP25QAIA3uHxXnzDPHZ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA21" s="8" t="s">
+      <c r="AA21" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC21" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2721,17 +3212,20 @@
         <v>AG_IV-M-A MICROECONOMÍA -</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S22,"' target='_blank'&gt;&lt;img src='",AC22,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/D9Sku7OhjYZKnx5enkubP5' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA22" s="8" t="s">
+      <c r="AA22" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC22" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB22" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2789,17 +3283,20 @@
         <v>AG_IV-T-B MICROECONOMÍA -</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S23,"' target='_blank'&gt;&lt;img src='",AC23,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/L1EyZjIafpfBnQojqWB3lX' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA23" s="8" t="s">
+      <c r="AA23" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC23" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2857,17 +3354,20 @@
         <v>AG_IV-M-A LIDERAZGO Y TRA</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S24,"' target='_blank'&gt;&lt;img src='",AC24,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GoMlxseRGhR9oncR3I7bYx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA24" s="8" t="s">
+      <c r="AA24" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC24" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2925,17 +3425,20 @@
         <v>AG_IV-T-B LIDERAZGO Y TRA</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S25,"' target='_blank'&gt;&lt;img src='",AC25,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CW75zbqAZcaL0K2sxpTR9f' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA25" s="8" t="s">
+      <c r="AA25" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC25" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2993,17 +3496,20 @@
         <v>AG_V-T-A MECANIZACIÓN AGR</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S26,"' target='_blank'&gt;&lt;img src='",AC26,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GTFAcBAcl0OACIv8D3NTWJ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA26" s="8" t="s">
+      <c r="AA26" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC26" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3061,17 +3567,20 @@
         <v>AG_V-T-A FISIOLOGÍA VEGET</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S27,"' target='_blank'&gt;&lt;img src='",AC27,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LB8RvogeZybAwAFswla07p' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA27" s="8" t="s">
+      <c r="AA27" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>303</v>
+      </c>
+      <c r="AC27" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB27" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3129,17 +3638,20 @@
         <v>AG_V-T-A GENÉTICA VEGETAL</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S28,"' target='_blank'&gt;&lt;img src='",AC28,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EqZyF07InkzI8lMRODGhqt' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA28" s="8" t="s">
+      <c r="AA28" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>305</v>
+      </c>
+      <c r="AC28" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3197,17 +3709,20 @@
         <v>AG_V-T-A METEOROLOGÍA - 2</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S29,"' target='_blank'&gt;&lt;img src='",AC29,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/L7RZY624mfWEq9tlMvTIus' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA29" s="8" t="s">
+      <c r="AA29" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC29" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3265,17 +3780,20 @@
         <v xml:space="preserve">AG_V-T-A MICROBIOLOGÍA - </v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S30,"' target='_blank'&gt;&lt;img src='",AC30,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GvjqkPjCddhBEfxEUIC9cd' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA30" s="8" t="s">
+      <c r="AA30" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>309</v>
+      </c>
+      <c r="AC30" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB30" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3333,17 +3851,20 @@
         <v>AG_V-T-A CONSTITUCIÓN Y D</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S31,"' target='_blank'&gt;&lt;img src='",AC31,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LkqH1O12bih2sPLsNSEAKQ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA31" s="8" t="s">
+      <c r="AA31" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>311</v>
+      </c>
+      <c r="AC31" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3401,17 +3922,20 @@
         <v>AG_V-T-A EDAFOLOGIA - 279</v>
       </c>
       <c r="Z32" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S32,"' target='_blank'&gt;&lt;img src='",AC32,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/D3dfgSaG1Dg1TYKWu2FYTZ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA32" s="8" t="s">
+      <c r="AA32" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>313</v>
+      </c>
+      <c r="AC32" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3469,17 +3993,20 @@
         <v>AG_VI-T-A AGROTECNÍA - 27</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S33,"' target='_blank'&gt;&lt;img src='",AC33,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KxqeMXxJ0o66axewKCLLET' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA33" s="8" t="s">
+      <c r="AA33" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>315</v>
+      </c>
+      <c r="AC33" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3537,17 +4064,20 @@
         <v xml:space="preserve">AG_VI-T-A FERTILIDAD DEL </v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S34,"' target='_blank'&gt;&lt;img src='",AC34,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JNFeaFVMeM6BPs4th2or1x' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA34" s="8" t="s">
+      <c r="AA34" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC34" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB34" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3605,17 +4135,20 @@
         <v xml:space="preserve">AG_VI-T-A PROPAGACIÓN DE </v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S35,"' target='_blank'&gt;&lt;img src='",AC35,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LrCGWON0GJm0C5YBRV2syV' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA35" s="8" t="s">
+      <c r="AA35" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>319</v>
+      </c>
+      <c r="AC35" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB35" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3673,17 +4206,20 @@
         <v>AG_VI-T-A ENTOMOLOGÍA GEN</v>
       </c>
       <c r="Z36" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S36,"' target='_blank'&gt;&lt;img src='",AC36,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FSkvKlBsg178BIszfbPGCe' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA36" s="8" t="s">
+      <c r="AA36" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC36" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3741,17 +4277,20 @@
         <v>AG_VI-T-A TOPOGRAFÍA - 27</v>
       </c>
       <c r="Z37" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S37,"' target='_blank'&gt;&lt;img src='",AC37,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JMt54zSVtWjJj4aun2gTeP' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA37" s="8" t="s">
+      <c r="AA37" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC37" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB37" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3809,17 +4348,20 @@
         <v>AG_VI-T-A PENSAMIENTO POL</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S38,"' target='_blank'&gt;&lt;img src='",AC38,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CAD7FpzLKqfEvhLi2JGLBC' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA38" s="8" t="s">
+      <c r="AA38" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>325</v>
+      </c>
+      <c r="AC38" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB38" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3877,17 +4419,20 @@
         <v>AG_VIII-M-A RAICES Y TUBÉ</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S39,"' target='_blank'&gt;&lt;img src='",AC39,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DJb4k4cxVtGGo9knbYaGfw' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA39" s="8" t="s">
+      <c r="AA39" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC39" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB39" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3945,17 +4490,20 @@
         <v>AG_VIII-T-B RAICES Y TUBÉ</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S40,"' target='_blank'&gt;&lt;img src='",AC40,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FbEHKnnVVplGAUteWC6n4P' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA40" s="8" t="s">
+      <c r="AA40" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>329</v>
+      </c>
+      <c r="AC40" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB40" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4013,17 +4561,20 @@
         <v xml:space="preserve">AG_VIII-M-A OLERICULTURA </v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S41,"' target='_blank'&gt;&lt;img src='",AC41,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/K02XA3agKfbFtuyGqV2g5q' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA41" s="8" t="s">
+      <c r="AA41" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>331</v>
+      </c>
+      <c r="AC41" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB41" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4081,17 +4632,20 @@
         <v xml:space="preserve">AG_VIII-T-B OLERICULTURA </v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S42,"' target='_blank'&gt;&lt;img src='",AC42,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J4GDbtVXLdJ4wwcu6wNXls' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA42" s="8" t="s">
+      <c r="AA42" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>333</v>
+      </c>
+      <c r="AC42" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB42" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4149,17 +4703,20 @@
         <v xml:space="preserve">AG_VIII-M-A FRUTICULTURA </v>
       </c>
       <c r="Z43" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S43,"' target='_blank'&gt;&lt;img src='",AC43,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Hl9vlkN6Tcc0W5Gv3ek4CK' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA43" s="8" t="s">
+      <c r="AA43" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>335</v>
+      </c>
+      <c r="AC43" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4217,17 +4774,20 @@
         <v xml:space="preserve">AG_VIII-T-B FRUTICULTURA </v>
       </c>
       <c r="Z44" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S44,"' target='_blank'&gt;&lt;img src='",AC44,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Hkdo8BCbdYF0r7lK0zDcx0' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA44" s="8" t="s">
+      <c r="AA44" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>337</v>
+      </c>
+      <c r="AC44" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB44" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4285,17 +4845,20 @@
         <v>AG_VIII-M-A ENTOMOLOGÍA A</v>
       </c>
       <c r="Z45" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S45,"' target='_blank'&gt;&lt;img src='",AC45,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BSjyRn0v7Hd0RZAwKDelHI' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA45" s="8" t="s">
+      <c r="AA45" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC45" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB45" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4353,17 +4916,20 @@
         <v>AG_VIII-T-B ENTOMOLOGÍA A</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S46,"' target='_blank'&gt;&lt;img src='",AC46,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/K1mkJtwQJheK0xmAS0WQ95' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA46" s="8" t="s">
+      <c r="AA46" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC46" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB46" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4421,17 +4987,20 @@
         <v>AG_VIII-M-A METODOLOGÍA D</v>
       </c>
       <c r="Z47" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S47,"' target='_blank'&gt;&lt;img src='",AC47,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DHQUOVl6iAN93UzdOo3ipP' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA47" s="8" t="s">
+      <c r="AA47" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>343</v>
+      </c>
+      <c r="AC47" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB47" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4489,17 +5058,20 @@
         <v>AG_VIII-T-B METODOLOGÍA D</v>
       </c>
       <c r="Z48" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S48,"' target='_blank'&gt;&lt;img src='",AC48,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EuhBbZ2mUVELCseDu0pCgA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA48" s="8" t="s">
+      <c r="AA48" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC48" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB48" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4557,17 +5129,20 @@
         <v>AG_VIII-M-A PRODUCCIÓN DE</v>
       </c>
       <c r="Z49" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S49,"' target='_blank'&gt;&lt;img src='",AC49,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Gs9BoN9Rtu01X277ysceDD' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA49" s="8" t="s">
+      <c r="AA49" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC49" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB49" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4625,17 +5200,20 @@
         <v>AG_VIII-T-B PRODUCCIÓN DE</v>
       </c>
       <c r="Z50" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S50,"' target='_blank'&gt;&lt;img src='",AC50,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EXaZtVMPIOxAZeyWFXg21A' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA50" s="8" t="s">
+      <c r="AA50" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC50" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB50" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4693,17 +5271,20 @@
         <v>AG_X-M-A FORMULACIÓN Y EV</v>
       </c>
       <c r="Z51" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S51,"' target='_blank'&gt;&lt;img src='",AC51,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FNJFXk5PFtyK2OP4LPVBP8' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA51" s="8" t="s">
+      <c r="AA51" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC51" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB51" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4761,17 +5342,20 @@
         <v>AG_X-T-B FORMULACIÓN Y EV</v>
       </c>
       <c r="Z52" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S52,"' target='_blank'&gt;&lt;img src='",AC52,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Cc6suyo0sVg7rzH29f1xNY' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA52" s="8" t="s">
+      <c r="AA52" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC52" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB52" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4829,17 +5413,20 @@
         <v>AG_X-M-A EXTENSIÓN AGRARI</v>
       </c>
       <c r="Z53" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S53,"' target='_blank'&gt;&lt;img src='",AC53,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EC78puZGT5G9RVgwd6G4Y3' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA53" s="8" t="s">
+      <c r="AA53" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>355</v>
+      </c>
+      <c r="AC53" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB53" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4897,17 +5484,20 @@
         <v>AG_X-T-B EXTENSIÓN AGRARI</v>
       </c>
       <c r="Z54" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S54,"' target='_blank'&gt;&lt;img src='",AC54,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FEAScn7L5txEH8ePcre5Rx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA54" s="8" t="s">
+      <c r="AA54" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>357</v>
+      </c>
+      <c r="AC54" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB54" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4965,17 +5555,20 @@
         <v>AG_X-M-A MANEJO INTEGRADO</v>
       </c>
       <c r="Z55" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S55,"' target='_blank'&gt;&lt;img src='",AC55,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J8mVfTRHEoC1V8nyMEIk56' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA55" s="8" t="s">
+      <c r="AA55" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC55" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB55" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5033,17 +5626,20 @@
         <v>AG_X-T-B MANEJO INTEGRADO</v>
       </c>
       <c r="Z56" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S56,"' target='_blank'&gt;&lt;img src='",AC56,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GOURuZSLUyr3hVVuHRLymg' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA56" s="8" t="s">
+      <c r="AA56" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>361</v>
+      </c>
+      <c r="AC56" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB56" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5101,17 +5697,20 @@
         <v>AG_X-M-A SEMINARIO DE TES</v>
       </c>
       <c r="Z57" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S57,"' target='_blank'&gt;&lt;img src='",AC57,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CXwOXFiDI10CwNgEz0axhc' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA57" s="8" t="s">
+      <c r="AA57" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>363</v>
+      </c>
+      <c r="AC57" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB57" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5169,17 +5768,20 @@
         <v>AG_X-T-B SEMINARIO DE TES</v>
       </c>
       <c r="Z58" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S58,"' target='_blank'&gt;&lt;img src='",AC58,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J1wt04kGjN89WKPhT7XmLf' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA58" s="8" t="s">
+      <c r="AA58" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>365</v>
+      </c>
+      <c r="AC58" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB58" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5237,17 +5839,20 @@
         <v>AG_X-M-A NUTRICIÓN Y ALIM</v>
       </c>
       <c r="Z59" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S59,"' target='_blank'&gt;&lt;img src='",AC59,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IqffUMSFMCpFLYeOhWsySp' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA59" s="8" t="s">
+      <c r="AA59" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC59" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB59" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5305,17 +5910,20 @@
         <v>AG_X-T-B NUTRICIÓN Y ALIM</v>
       </c>
       <c r="Z60" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S60,"' target='_blank'&gt;&lt;img src='",AC60,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IPQiyFFNNjpB3Fkgg3b0ZJ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA60" s="8" t="s">
+      <c r="AA60" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>369</v>
+      </c>
+      <c r="AC60" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB60" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5373,17 +5981,20 @@
         <v>AG_X-M-A CONTROL BIOLÓGIC</v>
       </c>
       <c r="Z61" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S61,"' target='_blank'&gt;&lt;img src='",AC61,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Ev0qZ2cGlfxAY7oKZvU0Wb' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA61" s="8" t="s">
+      <c r="AA61" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC61" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB61" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5441,17 +6052,20 @@
         <v>AG_X-T-B CONTROL BIOLÓGIC</v>
       </c>
       <c r="Z62" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S62,"' target='_blank'&gt;&lt;img src='",AC62,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Kwo6hH8eEQ9CBJzEcjLmbX' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA62" s="8" t="s">
+      <c r="AA62" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>372</v>
+      </c>
+      <c r="AC62" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB62" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5509,17 +6123,20 @@
         <v>AG_X-M-A AGRICULTURA ORGÁ</v>
       </c>
       <c r="Z63" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S63,"' target='_blank'&gt;&lt;img src='",AC63,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JkjOSwZ5t5d7mMPwQo9bha' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA63" s="8" t="s">
+      <c r="AA63" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>374</v>
+      </c>
+      <c r="AC63" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB63" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5574,17 +6191,20 @@
         <v>AG_X-T-B AGRICULTURA ORGÁ</v>
       </c>
       <c r="Z64" t="str">
-        <f t="shared" si="9"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S64,"' target='_blank'&gt;&lt;img src='",AC64,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KFYFa47lVAB0TvkCAxJOfx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA64" s="8" t="s">
+      <c r="AA64" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>376</v>
+      </c>
+      <c r="AC64" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="AB64" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>14</v>
       </c>
@@ -5595,10 +6215,10 @@
         <v>9</v>
       </c>
       <c r="D65" t="s">
+        <v>236</v>
+      </c>
+      <c r="E65" t="s">
         <v>237</v>
-      </c>
-      <c r="E65" t="s">
-        <v>238</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
@@ -5610,43 +6230,49 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U65" t="str">
         <f t="shared" si="4"/>
         <v>1150</v>
       </c>
       <c r="V65" t="str">
-        <f t="shared" ref="V65:V66" si="10">MID(D65,1,10)</f>
+        <f t="shared" ref="V65:V66" si="9">MID(D65,1,10)</f>
         <v>AG36 - 566</v>
       </c>
       <c r="W65" t="str">
-        <f t="shared" ref="W65:W66" si="11">TRIM(MID(D65,14,222))</f>
+        <f t="shared" ref="W65:W66" si="10">TRIM(MID(D65,14,222))</f>
         <v>MATEMÁTICA II - 2850</v>
       </c>
       <c r="X65" t="str">
-        <f t="shared" ref="X65:X66" si="12">CONCATENATE(B65,"_",E65,"-",F65,"-",G65," ",W65)</f>
+        <f t="shared" ref="X65:X66" si="11">CONCATENATE(B65,"_",E65,"-",F65,"-",G65," ",W65)</f>
         <v>AG_III-M-A MATEMÁTICA II - 2850</v>
       </c>
       <c r="Y65" t="str">
-        <f t="shared" ref="Y65:Y66" si="13">MID(X65,1,25)</f>
+        <f t="shared" ref="Y65:Y66" si="12">MID(X65,1,25)</f>
         <v xml:space="preserve">AG_III-M-A MATEMÁTICA II </v>
       </c>
       <c r="Z65" t="str">
-        <f t="shared" ref="Z65:Z66" si="14">CONCATENATE("&lt;p&gt;&lt;a href='",S65,"' target='_blank'&gt;&lt;img src='",AA65,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S65,"' target='_blank'&gt;&lt;img src='",AC65,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/H8JTCbxGrMAEgkdI38jH6F' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA65" s="8" t="s">
+      <c r="AA65" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC65" s="8" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1</v>
       </c>
@@ -5657,10 +6283,10 @@
         <v>9</v>
       </c>
       <c r="D66" t="s">
+        <v>239</v>
+      </c>
+      <c r="E66" t="s">
         <v>240</v>
-      </c>
-      <c r="E66" t="s">
-        <v>241</v>
       </c>
       <c r="F66" t="s">
         <v>9</v>
@@ -5672,43 +6298,49 @@
         <v>34</v>
       </c>
       <c r="I66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U66" t="str">
         <f t="shared" si="4"/>
         <v>1149</v>
       </c>
       <c r="V66" t="str">
+        <f t="shared" si="9"/>
+        <v>CB.1 - 677</v>
+      </c>
+      <c r="W66" t="str">
         <f t="shared" si="10"/>
-        <v>CB.1 - 677</v>
-      </c>
-      <c r="W66" t="str">
+        <v>MATEMÁTICA BÁSICA - 2849</v>
+      </c>
+      <c r="X66" t="str">
         <f t="shared" si="11"/>
-        <v>MATEMÁTICA BÁSICA - 2849</v>
-      </c>
-      <c r="X66" t="str">
+        <v>AG_I-M-A MATEMÁTICA BÁSICA - 2849</v>
+      </c>
+      <c r="Y66" t="str">
         <f t="shared" si="12"/>
-        <v>AG_I-M-A MATEMÁTICA BÁSICA - 2849</v>
-      </c>
-      <c r="Y66" t="str">
-        <f t="shared" si="13"/>
         <v>AG_I-M-A MATEMÁTICA BÁSIC</v>
       </c>
       <c r="Z66" t="str">
-        <f t="shared" si="14"/>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S66,"' target='_blank'&gt;&lt;img src='",AC66,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/C9Ncjfw6CxfDZfS5Z4ngkh' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA66" s="8" t="s">
+      <c r="AA66" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>380</v>
+      </c>
+      <c r="AC66" s="8" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>25</v>
       </c>
@@ -5716,7 +6348,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E67" t="s">
         <v>18</v>
@@ -5728,36 +6360,42 @@
         <v>11</v>
       </c>
       <c r="I67" t="s">
+        <v>245</v>
+      </c>
+      <c r="T67" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="T67" s="9" t="s">
-        <v>247</v>
-      </c>
       <c r="U67" t="str">
-        <f t="shared" ref="U67" si="15">MID(T67,45,4)</f>
+        <f t="shared" ref="U67" si="13">MID(T67,45,4)</f>
         <v>1162</v>
       </c>
       <c r="V67" t="str">
-        <f t="shared" ref="V67" si="16">MID(D67,1,10)</f>
+        <f t="shared" ref="V67" si="14">MID(D67,1,10)</f>
         <v>AG56 - 611</v>
       </c>
       <c r="W67" t="str">
-        <f t="shared" ref="W67" si="17">TRIM(MID(D67,14,222))</f>
+        <f t="shared" ref="W67" si="15">TRIM(MID(D67,14,222))</f>
         <v>EDAFOLOGIA - 2756</v>
       </c>
       <c r="X67" t="str">
-        <f t="shared" ref="X67" si="18">CONCATENATE(B67,"_",E67,"-",F67,"-",G67," ",W67)</f>
+        <f t="shared" ref="X67" si="16">CONCATENATE(B67,"_",E67,"-",F67,"-",G67," ",W67)</f>
         <v>AG_V-T-B EDAFOLOGIA - 2756</v>
       </c>
       <c r="Y67" t="str">
-        <f t="shared" ref="Y67" si="19">MID(X67,1,25)</f>
+        <f t="shared" ref="Y67" si="17">MID(X67,1,25)</f>
         <v>AG_V-T-B EDAFOLOGIA - 275</v>
       </c>
       <c r="Z67" t="str">
-        <f t="shared" ref="Z67" si="20">CONCATENATE("&lt;p&gt;&lt;a href='",S67,"' target='_blank'&gt;&lt;img src='",AA67,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S67,"' target='_blank'&gt;&lt;img src='",AC67,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
-      <c r="AA67" s="8" t="s">
+      <c r="AA67" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>382</v>
+      </c>
+      <c r="AC67" s="8" t="s">
         <v>234</v>
       </c>
     </row>
@@ -5765,9 +6403,75 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="T2" r:id="rId1" xr:uid="{206E1AA6-869D-4007-9046-156304C1C689}"/>
+    <hyperlink ref="AA2" r:id="rId2" xr:uid="{5308CB3C-38E6-45E6-AEB6-96B598C64F13}"/>
+    <hyperlink ref="AA3" r:id="rId3" xr:uid="{5A744694-52A9-43A9-8AEB-904A8D44F537}"/>
+    <hyperlink ref="AA4" r:id="rId4" xr:uid="{F2B60812-E2B3-4221-9688-E333FA839F12}"/>
+    <hyperlink ref="AA5" r:id="rId5" xr:uid="{A9A4096E-E559-4FDD-9D2B-EF41B25B25C7}"/>
+    <hyperlink ref="AA6" r:id="rId6" xr:uid="{E1335791-B69B-4FAA-9C9B-ED8581A87E52}"/>
+    <hyperlink ref="AA7" r:id="rId7" xr:uid="{649A07D4-3C86-4FBC-84EC-9C568108C30E}"/>
+    <hyperlink ref="AA8" r:id="rId8" xr:uid="{15635622-2746-4FD2-8595-8A1CBB30E9E3}"/>
+    <hyperlink ref="AA9" r:id="rId9" xr:uid="{BF3B7B0B-730C-4A67-974F-42C91E3AF1F4}"/>
+    <hyperlink ref="AA10" r:id="rId10" xr:uid="{9EE1958E-6AF5-454F-9070-601247B8EDBC}"/>
+    <hyperlink ref="AA11" r:id="rId11" xr:uid="{713E8DDF-A11B-42DC-A4EB-E00ACF0740B0}"/>
+    <hyperlink ref="AA12" r:id="rId12" xr:uid="{EEA065E0-3276-4601-9001-75C1B2C161C0}"/>
+    <hyperlink ref="AA13" r:id="rId13" xr:uid="{DDB61E63-0842-4CED-A60E-CF216DFA285C}"/>
+    <hyperlink ref="AA14" r:id="rId14" xr:uid="{2F4E98D7-4BF6-4646-8F59-304E109099E7}"/>
+    <hyperlink ref="AA15" r:id="rId15" xr:uid="{D2686A27-CD89-4407-B5D1-8479236B412A}"/>
+    <hyperlink ref="AA16" r:id="rId16" xr:uid="{0CB51F4E-D1A6-4E1E-96A5-524F0E513B1F}"/>
+    <hyperlink ref="AA17" r:id="rId17" xr:uid="{67621535-84AF-432C-BC57-25C225449B49}"/>
+    <hyperlink ref="AA18" r:id="rId18" xr:uid="{616CEAE7-1A24-4D44-B9F4-064E33A72705}"/>
+    <hyperlink ref="AA19" r:id="rId19" xr:uid="{47C763F2-58E6-4F03-91CC-0C4B222FD0B1}"/>
+    <hyperlink ref="AA20" r:id="rId20" xr:uid="{5093E5B6-483B-4245-9E34-8FD6087DE456}"/>
+    <hyperlink ref="AA21" r:id="rId21" xr:uid="{363DAF0E-2E79-4FD7-B635-3951552E8EBB}"/>
+    <hyperlink ref="AA22" r:id="rId22" xr:uid="{0B28DF84-D365-445F-992A-4167DF179046}"/>
+    <hyperlink ref="AA23" r:id="rId23" xr:uid="{28A6B91D-7770-4223-B8DC-AF75A9EC4CDA}"/>
+    <hyperlink ref="AA24" r:id="rId24" xr:uid="{0DC78A6D-2075-441A-8BA7-91D3E4E8D101}"/>
+    <hyperlink ref="AA25" r:id="rId25" xr:uid="{8039BB07-8976-4F5F-A637-B350C4416485}"/>
+    <hyperlink ref="AA26" r:id="rId26" xr:uid="{C055D3BA-F739-4B9F-B9FE-D50B58FEE6D9}"/>
+    <hyperlink ref="AA27" r:id="rId27" xr:uid="{5D6B8C24-C057-417D-A2C2-BB0B187A8286}"/>
+    <hyperlink ref="AA28" r:id="rId28" xr:uid="{27602E7B-426B-4B67-9ABE-C8AFB0BC242C}"/>
+    <hyperlink ref="AA29" r:id="rId29" xr:uid="{FC8C6A88-5576-4C69-BFB8-96A04BC671CB}"/>
+    <hyperlink ref="AA30" r:id="rId30" xr:uid="{138D68E4-03C5-4A8B-8515-161A66100491}"/>
+    <hyperlink ref="AA31" r:id="rId31" xr:uid="{25A53A91-7706-4E47-93C4-73B8221B712C}"/>
+    <hyperlink ref="AA32" r:id="rId32" xr:uid="{039A863A-16F3-44AE-BDB3-C85290715BE4}"/>
+    <hyperlink ref="AA33" r:id="rId33" xr:uid="{3ACC6554-F64D-4DAF-83E9-10764CF4EF6F}"/>
+    <hyperlink ref="AA34" r:id="rId34" xr:uid="{607BEC07-D2C1-41D1-9E3E-008C183FECBB}"/>
+    <hyperlink ref="AA35" r:id="rId35" xr:uid="{D931A5C1-32A8-4641-8EC4-3836C2D80208}"/>
+    <hyperlink ref="AA36" r:id="rId36" xr:uid="{51B876EE-7B96-404A-8A36-3C4EBC8A28FD}"/>
+    <hyperlink ref="AA37" r:id="rId37" xr:uid="{5F526F7F-2E28-41A5-BE47-A64518F1BF2E}"/>
+    <hyperlink ref="AA38" r:id="rId38" xr:uid="{A9F6EB40-7D49-4D08-93F0-F46D81FD1421}"/>
+    <hyperlink ref="AA39" r:id="rId39" xr:uid="{58EB9EB7-CCAC-4780-977F-8FDB150106E7}"/>
+    <hyperlink ref="AA40" r:id="rId40" xr:uid="{F422FC0E-20EB-460C-BDFB-12261B0D0CC6}"/>
+    <hyperlink ref="AA41" r:id="rId41" xr:uid="{CF61DCC4-303D-4A25-8CB3-2DDE9E82A9BE}"/>
+    <hyperlink ref="AA42" r:id="rId42" xr:uid="{235700EA-8B97-4D05-B0DC-356251FFA966}"/>
+    <hyperlink ref="AA43" r:id="rId43" xr:uid="{96E62F7A-A225-44BA-8C68-B2002709760A}"/>
+    <hyperlink ref="AA44" r:id="rId44" xr:uid="{F3A8B14F-B052-4CC4-80C7-5B355869853D}"/>
+    <hyperlink ref="AA45" r:id="rId45" xr:uid="{56685AB2-00B6-4DBA-ADCD-4240F8B8DAEF}"/>
+    <hyperlink ref="AA46" r:id="rId46" xr:uid="{5575BEDE-1E7F-4A64-8B9A-9132CC281DE0}"/>
+    <hyperlink ref="AA47" r:id="rId47" xr:uid="{32EB3FD7-91EC-471A-A5BA-2F2D3E2AE802}"/>
+    <hyperlink ref="AA48" r:id="rId48" xr:uid="{99F3A4D4-C32E-4808-A289-55A5FE4010D0}"/>
+    <hyperlink ref="AA49" r:id="rId49" xr:uid="{6A1571D0-6B75-4E6D-9F61-6061890A597D}"/>
+    <hyperlink ref="AA50" r:id="rId50" xr:uid="{D5BD23BD-A4A7-45AA-9910-94DC6814FEEF}"/>
+    <hyperlink ref="AA51" r:id="rId51" xr:uid="{2C09063E-C805-4DDB-A606-22A8916052EE}"/>
+    <hyperlink ref="AA52" r:id="rId52" xr:uid="{95D2BC0F-3025-4B08-918B-5FE0936FD99B}"/>
+    <hyperlink ref="AA53" r:id="rId53" xr:uid="{E0B00368-1DCB-4493-B404-56DD1CA0B892}"/>
+    <hyperlink ref="AA54" r:id="rId54" xr:uid="{9AB0BB1A-34AE-4EEB-BDED-1CAB8D3E9EEA}"/>
+    <hyperlink ref="AA55" r:id="rId55" xr:uid="{2D930515-89D1-4CA7-93A3-4A4CEA0D5FD7}"/>
+    <hyperlink ref="AA56" r:id="rId56" xr:uid="{C68CA293-2612-40D6-9EE8-A1B701BE8511}"/>
+    <hyperlink ref="AA57" r:id="rId57" xr:uid="{3DF3FA19-75C9-480A-99B0-A2431322064B}"/>
+    <hyperlink ref="AA58" r:id="rId58" xr:uid="{4D673175-D57C-425E-A91E-D59EDAF8FB5A}"/>
+    <hyperlink ref="AA59" r:id="rId59" xr:uid="{0C0EFDD0-9D1E-4775-B624-D13FCF9BAF86}"/>
+    <hyperlink ref="AA60" r:id="rId60" xr:uid="{A807F9C3-5585-442F-B571-FBEC5DCFDE52}"/>
+    <hyperlink ref="AA61" r:id="rId61" xr:uid="{CC9473D1-B265-4BE4-97C6-163AE513290A}"/>
+    <hyperlink ref="AA62" r:id="rId62" xr:uid="{AAF2925F-AADF-485E-AB37-B63DD3B8CEA2}"/>
+    <hyperlink ref="AA63" r:id="rId63" xr:uid="{8F599692-1420-4261-AEE3-194612FD311C}"/>
+    <hyperlink ref="AA64" r:id="rId64" xr:uid="{FCD7EF14-AE94-4CC9-AD5F-636F9FDA7F81}"/>
+    <hyperlink ref="AA65" r:id="rId65" xr:uid="{CF329BFF-4D3B-4C2C-A73D-88394D7CA890}"/>
+    <hyperlink ref="AA66" r:id="rId66" xr:uid="{4B1955D4-97E0-45D8-8F96-3BFB41682321}"/>
+    <hyperlink ref="AA67" r:id="rId67" xr:uid="{DBE3B756-F5AB-43B8-99AF-0F18BDBA4962}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -5787,7 +6491,7 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update create and delete group whatsapp, aula virtual tag link group whatsapp, matricula masiva
</commit_message>
<xml_diff>
--- a/grupowsp.xlsx
+++ b/grupowsp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9116F8-E3E8-4A09-A630-1813B82629FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A8F4DA-C8EE-4068-9398-FC181ED69FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="885" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="446">
   <si>
     <t>N°</t>
   </si>
@@ -728,9 +728,6 @@
     <t>https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5</t>
   </si>
   <si>
-    <t>&lt;span role='presentation' style='padding-right: 0.1px'&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
     <t>AG36 - 566 - MATEMÁTICA II - 2850</t>
   </si>
   <si>
@@ -1170,6 +1167,198 @@
   </si>
   <si>
     <t>484.4MB</t>
+  </si>
+  <si>
+    <t>AG_II-M-A CULTURA AMBIENT 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B CULTURA AMBIENT 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-M-A ANÁLISIS MATEMÁ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B ANÁLISIS MATEMÁ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-M-A QUÍMICA GENERAL 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B QUÍMICA GENERAL 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-M-A BOTÁNICA GENERA 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B BOTÁNICA GENERA 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-M-A INFORMÁTICA - 2 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B INFORMÁTICA - 2 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A BIOQUÍMICA GENE 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A ESTADÍSTICA GEN 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B ESTADÍSTICA GEN 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A FÍSICA II - 277 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B FÍSICA II - 278 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A MICROECONOMÍA - 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B MICROECONOMÍA - 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A LIDERAZGO Y TRA 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B LIDERAZGO Y TRA 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A MECANIZACIÓN AGR 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A FISIOLOGÍA VEGET 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A GENÉTICA VEGETAL 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A METEOROLOGÍA - 2 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A CONSTITUCIÓN Y D 1 participante</t>
+  </si>
+  <si>
+    <t>AG_V-T-A EDAFOLOGIA - 279 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A AGROTECNÍA - 27 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A ENTOMOLOGÍA GEN 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A PENSAMIENTO POL 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A RAICES Y TUBÉ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B RAICES Y TUBÉ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A ENTOMOLOGÍA A 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B ENTOMOLOGÍA A 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B METODOLOGÍA D 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A PRODUCCIÓN DE 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B PRODUCCIÓN DE 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A FORMULACIÓN Y EV 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B FORMULACIÓN Y EV 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A EXTENSIÓN AGRARI 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B EXTENSIÓN AGRARI 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A MANEJO INTEGRADO 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B MANEJO INTEGRADO 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A SEMINARIO DE TES 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B SEMINARIO DE TES 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A NUTRICIÓN Y ALIM 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B NUTRICIÓN Y ALIM 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A CONTROL BIOLÓGIC 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-M-A FÍSICA - 2764 1 participante</t>
+  </si>
+  <si>
+    <t>AG_II-T-B FÍSICA - 2770 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B BIOQUÍMICA GENE 1 participante</t>
+  </si>
+  <si>
+    <t>AG_IV-M-A AGROECOLOGÍA - 32 participantes</t>
+  </si>
+  <si>
+    <t>AG_IV-T-B AGROECOLOGÍA - 29 participantes</t>
+  </si>
+  <si>
+    <t>AG_V-T-A MICROBIOLOGÍA - 38 participantes</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A FERTILIDAD DEL 37 participantes</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A PROPAGACIÓN DE 36 participantes</t>
+  </si>
+  <si>
+    <t>AG_VI-T-A TOPOGRAFÍA - 27 1 participante</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A OLERICULTURA 26 participantes</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B OLERICULTURA 25 participantes</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A FRUTICULTURA 31 participantes</t>
+  </si>
+  <si>
+    <t>AG_VIII-T-B FRUTICULTURA 32 participantes</t>
+  </si>
+  <si>
+    <t>AG_VIII-M-A METODOLOGÍA D 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B CONTROL BIOLÓGIC 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-M-A AGRICULTURA ORGÁ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_X-T-B AGRICULTURA ORGÁ 1 participante</t>
+  </si>
+  <si>
+    <t>AG_III-M-A MATEMÁTICA II 48 participantes</t>
   </si>
 </sst>
 </file>
@@ -1641,9 +1830,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1710,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="U1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V1" s="5" t="s">
         <v>2</v>
@@ -1728,10 +1917,10 @@
         <v>7</v>
       </c>
       <c r="AA1" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>250</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -1788,18 +1977,18 @@
         <v>AG_II-M-A CULTURA AMBIENTAL - 2767</v>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2" si="3">MID(X2,1,25)</f>
+        <f>TRIM(MID(X2,1,25))</f>
         <v>AG_II-M-A CULTURA AMBIENT</v>
       </c>
       <c r="Z2" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S2,"' target='_blank'&gt;&lt;img src='",AC2,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" ref="Z2:Z33" si="3">CONCATENATE("&lt;p&gt;&lt;a href='",S2,"' target='_blank'&gt;&lt;img src='",AC2,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LWJSKSqib1fH6uocU35PYb' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA2" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB2" t="s">
         <v>252</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>253</v>
       </c>
       <c r="AC2" s="8" t="s">
         <v>234</v>
@@ -1859,18 +2048,18 @@
         <v>AG_II-T-B CULTURA AMBIENTAL - 2773</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y64" si="8">MID(X3,1,25)</f>
+        <f t="shared" ref="Y3:Y66" si="8">TRIM(MID(X3,1,25))</f>
         <v>AG_II-T-B CULTURA AMBIENT</v>
       </c>
       <c r="Z3" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S3,"' target='_blank'&gt;&lt;img src='",AC3,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JWMiL8dNxPQ642NljMskFw' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA3" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB3" t="s">
         <v>254</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>255</v>
       </c>
       <c r="AC3" s="8" t="s">
         <v>234</v>
@@ -1934,14 +2123,14 @@
         <v>AG_II-M-A ANÁLISIS MATEMÁ</v>
       </c>
       <c r="Z4" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S4,"' target='_blank'&gt;&lt;img src='",AC4,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BVsq7GvIbpzLPDxWuh9RXx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA4" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB4" t="s">
         <v>256</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>257</v>
       </c>
       <c r="AC4" s="8" t="s">
         <v>234</v>
@@ -2005,14 +2194,14 @@
         <v>AG_II-T-B ANÁLISIS MATEMÁ</v>
       </c>
       <c r="Z5" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S5,"' target='_blank'&gt;&lt;img src='",AC5,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CnT9oBWGpph5yKj8Nfz5c5' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA5" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB5" t="s">
         <v>258</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>259</v>
       </c>
       <c r="AC5" s="8" t="s">
         <v>234</v>
@@ -2076,14 +2265,14 @@
         <v>AG_II-M-A FÍSICA - 2764</v>
       </c>
       <c r="Z6" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S6,"' target='_blank'&gt;&lt;img src='",AC6,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/HsXEKyk5ZOLFDK4Y4GWwLA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA6" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB6" t="s">
         <v>260</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>261</v>
       </c>
       <c r="AC6" s="8" t="s">
         <v>234</v>
@@ -2147,14 +2336,14 @@
         <v>AG_II-T-B FÍSICA - 2770</v>
       </c>
       <c r="Z7" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S7,"' target='_blank'&gt;&lt;img src='",AC7,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CfAVpDRlBdX4E1zem4qrEn' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA7" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB7" t="s">
         <v>262</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>263</v>
       </c>
       <c r="AC7" s="8" t="s">
         <v>234</v>
@@ -2218,14 +2407,14 @@
         <v>AG_II-M-A QUÍMICA GENERAL</v>
       </c>
       <c r="Z8" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S8,"' target='_blank'&gt;&lt;img src='",AC8,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IOUAT3LwFHCA0Fr2PrS7Ui' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA8" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB8" t="s">
         <v>264</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>265</v>
       </c>
       <c r="AC8" s="8" t="s">
         <v>234</v>
@@ -2289,14 +2478,14 @@
         <v>AG_II-T-B QUÍMICA GENERAL</v>
       </c>
       <c r="Z9" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S9,"' target='_blank'&gt;&lt;img src='",AC9,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KtuxNltmEqWDFhw2RVnVho' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA9" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB9" t="s">
         <v>266</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>267</v>
       </c>
       <c r="AC9" s="8" t="s">
         <v>234</v>
@@ -2360,14 +2549,14 @@
         <v>AG_II-M-A BOTÁNICA GENERA</v>
       </c>
       <c r="Z10" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S10,"' target='_blank'&gt;&lt;img src='",AC10,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KPsHkXMLMet6faBGdSZQex' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA10" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="AB10" t="s">
         <v>268</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>269</v>
       </c>
       <c r="AC10" s="8" t="s">
         <v>234</v>
@@ -2431,14 +2620,14 @@
         <v>AG_II-T-B BOTÁNICA GENERA</v>
       </c>
       <c r="Z11" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S11,"' target='_blank'&gt;&lt;img src='",AC11,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J0LEUV90FrjJX778c2ietI' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA11" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB11" t="s">
         <v>270</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>271</v>
       </c>
       <c r="AC11" s="8" t="s">
         <v>234</v>
@@ -2502,14 +2691,14 @@
         <v>AG_II-M-A INFORMÁTICA - 2</v>
       </c>
       <c r="Z12" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S12,"' target='_blank'&gt;&lt;img src='",AC12,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LiqhSZJoUyFDPPWBahSaXq' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA12" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB12" t="s">
         <v>272</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>273</v>
       </c>
       <c r="AC12" s="8" t="s">
         <v>234</v>
@@ -2573,14 +2762,14 @@
         <v>AG_II-T-B INFORMÁTICA - 2</v>
       </c>
       <c r="Z13" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S13,"' target='_blank'&gt;&lt;img src='",AC13,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CaWfkGJVannHNmr4bBlYaA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA13" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB13" t="s">
         <v>274</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>275</v>
       </c>
       <c r="AC13" s="8" t="s">
         <v>234</v>
@@ -2644,14 +2833,14 @@
         <v>AG_IV-M-A BIOQUÍMICA GENE</v>
       </c>
       <c r="Z14" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S14,"' target='_blank'&gt;&lt;img src='",AC14,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FF4MoK2k3Bp2JRfHWFtn2e' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA14" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB14" t="s">
         <v>276</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>277</v>
       </c>
       <c r="AC14" s="8" t="s">
         <v>234</v>
@@ -2715,14 +2904,14 @@
         <v>AG_IV-T-B BIOQUÍMICA GENE</v>
       </c>
       <c r="Z15" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S15,"' target='_blank'&gt;&lt;img src='",AC15,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Ikat0W4Vkjc9DOM8k1zrwa' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA15" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB15" t="s">
         <v>278</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>279</v>
       </c>
       <c r="AC15" s="8" t="s">
         <v>234</v>
@@ -2786,14 +2975,14 @@
         <v>AG_IV-M-A ESTADÍSTICA GEN</v>
       </c>
       <c r="Z16" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S16,"' target='_blank'&gt;&lt;img src='",AC16,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J7kjcXw4SeP6Lm2yB4s0Hd' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA16" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB16" t="s">
         <v>280</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>281</v>
       </c>
       <c r="AC16" s="8" t="s">
         <v>234</v>
@@ -2857,14 +3046,14 @@
         <v>AG_IV-T-B ESTADÍSTICA GEN</v>
       </c>
       <c r="Z17" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S17,"' target='_blank'&gt;&lt;img src='",AC17,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Jv66x356fa84eqiAZibbtB' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA17" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB17" t="s">
         <v>282</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>283</v>
       </c>
       <c r="AC17" s="8" t="s">
         <v>234</v>
@@ -2928,14 +3117,14 @@
         <v>AG_IV-M-A FÍSICA II - 277</v>
       </c>
       <c r="Z18" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S18,"' target='_blank'&gt;&lt;img src='",AC18,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DbzaveELGys0X6N50SABYq' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA18" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB18" t="s">
         <v>284</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>285</v>
       </c>
       <c r="AC18" s="8" t="s">
         <v>234</v>
@@ -2999,14 +3188,14 @@
         <v>AG_IV-T-B FÍSICA II - 278</v>
       </c>
       <c r="Z19" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S19,"' target='_blank'&gt;&lt;img src='",AC19,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BYJKAz8Qvkg6rgwCjQQYfm' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA19" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="AB19" t="s">
         <v>286</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>287</v>
       </c>
       <c r="AC19" s="8" t="s">
         <v>234</v>
@@ -3067,17 +3256,17 @@
       </c>
       <c r="Y20" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_IV-M-A AGROECOLOGÍA - </v>
+        <v>AG_IV-M-A AGROECOLOGÍA -</v>
       </c>
       <c r="Z20" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S20,"' target='_blank'&gt;&lt;img src='",AC20,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LrEwv8Dfv1Z1gYTj2DuKfo' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA20" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB20" t="s">
         <v>288</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>289</v>
       </c>
       <c r="AC20" s="8" t="s">
         <v>234</v>
@@ -3138,17 +3327,17 @@
       </c>
       <c r="Y21" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_IV-T-B AGROECOLOGÍA - </v>
+        <v>AG_IV-T-B AGROECOLOGÍA -</v>
       </c>
       <c r="Z21" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S21,"' target='_blank'&gt;&lt;img src='",AC21,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BojTP25QAIA3uHxXnzDPHZ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA21" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB21" t="s">
         <v>290</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>291</v>
       </c>
       <c r="AC21" s="8" t="s">
         <v>234</v>
@@ -3212,14 +3401,14 @@
         <v>AG_IV-M-A MICROECONOMÍA -</v>
       </c>
       <c r="Z22" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S22,"' target='_blank'&gt;&lt;img src='",AC22,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/D9Sku7OhjYZKnx5enkubP5' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA22" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB22" t="s">
         <v>292</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>293</v>
       </c>
       <c r="AC22" s="8" t="s">
         <v>234</v>
@@ -3283,14 +3472,14 @@
         <v>AG_IV-T-B MICROECONOMÍA -</v>
       </c>
       <c r="Z23" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S23,"' target='_blank'&gt;&lt;img src='",AC23,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/L1EyZjIafpfBnQojqWB3lX' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA23" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB23" t="s">
         <v>294</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>295</v>
       </c>
       <c r="AC23" s="8" t="s">
         <v>234</v>
@@ -3354,14 +3543,14 @@
         <v>AG_IV-M-A LIDERAZGO Y TRA</v>
       </c>
       <c r="Z24" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S24,"' target='_blank'&gt;&lt;img src='",AC24,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GoMlxseRGhR9oncR3I7bYx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA24" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB24" t="s">
         <v>296</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>297</v>
       </c>
       <c r="AC24" s="8" t="s">
         <v>234</v>
@@ -3425,14 +3614,14 @@
         <v>AG_IV-T-B LIDERAZGO Y TRA</v>
       </c>
       <c r="Z25" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S25,"' target='_blank'&gt;&lt;img src='",AC25,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CW75zbqAZcaL0K2sxpTR9f' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA25" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="AB25" t="s">
         <v>298</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>299</v>
       </c>
       <c r="AC25" s="8" t="s">
         <v>234</v>
@@ -3496,14 +3685,14 @@
         <v>AG_V-T-A MECANIZACIÓN AGR</v>
       </c>
       <c r="Z26" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S26,"' target='_blank'&gt;&lt;img src='",AC26,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GTFAcBAcl0OACIv8D3NTWJ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA26" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB26" t="s">
         <v>300</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>301</v>
       </c>
       <c r="AC26" s="8" t="s">
         <v>234</v>
@@ -3567,14 +3756,14 @@
         <v>AG_V-T-A FISIOLOGÍA VEGET</v>
       </c>
       <c r="Z27" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S27,"' target='_blank'&gt;&lt;img src='",AC27,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LB8RvogeZybAwAFswla07p' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA27" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="AB27" t="s">
         <v>302</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>303</v>
       </c>
       <c r="AC27" s="8" t="s">
         <v>234</v>
@@ -3638,14 +3827,14 @@
         <v>AG_V-T-A GENÉTICA VEGETAL</v>
       </c>
       <c r="Z28" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S28,"' target='_blank'&gt;&lt;img src='",AC28,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EqZyF07InkzI8lMRODGhqt' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA28" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="AB28" t="s">
         <v>304</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>305</v>
       </c>
       <c r="AC28" s="8" t="s">
         <v>234</v>
@@ -3709,14 +3898,14 @@
         <v>AG_V-T-A METEOROLOGÍA - 2</v>
       </c>
       <c r="Z29" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S29,"' target='_blank'&gt;&lt;img src='",AC29,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/L7RZY624mfWEq9tlMvTIus' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA29" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB29" t="s">
         <v>306</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>307</v>
       </c>
       <c r="AC29" s="8" t="s">
         <v>234</v>
@@ -3777,17 +3966,17 @@
       </c>
       <c r="Y30" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_V-T-A MICROBIOLOGÍA - </v>
+        <v>AG_V-T-A MICROBIOLOGÍA -</v>
       </c>
       <c r="Z30" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S30,"' target='_blank'&gt;&lt;img src='",AC30,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GvjqkPjCddhBEfxEUIC9cd' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA30" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="AB30" t="s">
         <v>308</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>309</v>
       </c>
       <c r="AC30" s="8" t="s">
         <v>234</v>
@@ -3851,14 +4040,14 @@
         <v>AG_V-T-A CONSTITUCIÓN Y D</v>
       </c>
       <c r="Z31" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S31,"' target='_blank'&gt;&lt;img src='",AC31,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LkqH1O12bih2sPLsNSEAKQ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA31" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB31" t="s">
         <v>310</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>311</v>
       </c>
       <c r="AC31" s="8" t="s">
         <v>234</v>
@@ -3922,14 +4111,14 @@
         <v>AG_V-T-A EDAFOLOGIA - 279</v>
       </c>
       <c r="Z32" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S32,"' target='_blank'&gt;&lt;img src='",AC32,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/D3dfgSaG1Dg1TYKWu2FYTZ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA32" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB32" t="s">
         <v>312</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>313</v>
       </c>
       <c r="AC32" s="8" t="s">
         <v>234</v>
@@ -3993,14 +4182,14 @@
         <v>AG_VI-T-A AGROTECNÍA - 27</v>
       </c>
       <c r="Z33" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S33,"' target='_blank'&gt;&lt;img src='",AC33,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="3"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KxqeMXxJ0o66axewKCLLET' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA33" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="AB33" t="s">
         <v>314</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>315</v>
       </c>
       <c r="AC33" s="8" t="s">
         <v>234</v>
@@ -4061,17 +4250,17 @@
       </c>
       <c r="Y34" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VI-T-A FERTILIDAD DEL </v>
+        <v>AG_VI-T-A FERTILIDAD DEL</v>
       </c>
       <c r="Z34" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S34,"' target='_blank'&gt;&lt;img src='",AC34,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" ref="Z34:Z67" si="9">CONCATENATE("&lt;p&gt;&lt;a href='",S34,"' target='_blank'&gt;&lt;img src='",AC34,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JNFeaFVMeM6BPs4th2or1x' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA34" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB34" t="s">
         <v>316</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>317</v>
       </c>
       <c r="AC34" s="8" t="s">
         <v>234</v>
@@ -4132,17 +4321,17 @@
       </c>
       <c r="Y35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VI-T-A PROPAGACIÓN DE </v>
+        <v>AG_VI-T-A PROPAGACIÓN DE</v>
       </c>
       <c r="Z35" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S35,"' target='_blank'&gt;&lt;img src='",AC35,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/LrCGWON0GJm0C5YBRV2syV' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA35" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB35" t="s">
         <v>318</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>319</v>
       </c>
       <c r="AC35" s="8" t="s">
         <v>234</v>
@@ -4206,14 +4395,14 @@
         <v>AG_VI-T-A ENTOMOLOGÍA GEN</v>
       </c>
       <c r="Z36" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S36,"' target='_blank'&gt;&lt;img src='",AC36,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FSkvKlBsg178BIszfbPGCe' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA36" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="AB36" t="s">
         <v>320</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>321</v>
       </c>
       <c r="AC36" s="8" t="s">
         <v>234</v>
@@ -4277,14 +4466,14 @@
         <v>AG_VI-T-A TOPOGRAFÍA - 27</v>
       </c>
       <c r="Z37" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S37,"' target='_blank'&gt;&lt;img src='",AC37,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JMt54zSVtWjJj4aun2gTeP' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA37" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB37" t="s">
         <v>322</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>323</v>
       </c>
       <c r="AC37" s="8" t="s">
         <v>234</v>
@@ -4348,14 +4537,14 @@
         <v>AG_VI-T-A PENSAMIENTO POL</v>
       </c>
       <c r="Z38" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S38,"' target='_blank'&gt;&lt;img src='",AC38,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CAD7FpzLKqfEvhLi2JGLBC' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA38" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB38" t="s">
         <v>324</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>325</v>
       </c>
       <c r="AC38" s="8" t="s">
         <v>234</v>
@@ -4419,14 +4608,14 @@
         <v>AG_VIII-M-A RAICES Y TUBÉ</v>
       </c>
       <c r="Z39" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S39,"' target='_blank'&gt;&lt;img src='",AC39,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DJb4k4cxVtGGo9knbYaGfw' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA39" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB39" t="s">
         <v>326</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>327</v>
       </c>
       <c r="AC39" s="8" t="s">
         <v>234</v>
@@ -4490,14 +4679,14 @@
         <v>AG_VIII-T-B RAICES Y TUBÉ</v>
       </c>
       <c r="Z40" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S40,"' target='_blank'&gt;&lt;img src='",AC40,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FbEHKnnVVplGAUteWC6n4P' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA40" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="AB40" t="s">
         <v>328</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>329</v>
       </c>
       <c r="AC40" s="8" t="s">
         <v>234</v>
@@ -4558,17 +4747,17 @@
       </c>
       <c r="Y41" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VIII-M-A OLERICULTURA </v>
+        <v>AG_VIII-M-A OLERICULTURA</v>
       </c>
       <c r="Z41" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S41,"' target='_blank'&gt;&lt;img src='",AC41,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/K02XA3agKfbFtuyGqV2g5q' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA41" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB41" t="s">
         <v>330</v>
-      </c>
-      <c r="AB41" t="s">
-        <v>331</v>
       </c>
       <c r="AC41" s="8" t="s">
         <v>234</v>
@@ -4629,17 +4818,17 @@
       </c>
       <c r="Y42" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VIII-T-B OLERICULTURA </v>
+        <v>AG_VIII-T-B OLERICULTURA</v>
       </c>
       <c r="Z42" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S42,"' target='_blank'&gt;&lt;img src='",AC42,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J4GDbtVXLdJ4wwcu6wNXls' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA42" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="AB42" t="s">
         <v>332</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>333</v>
       </c>
       <c r="AC42" s="8" t="s">
         <v>234</v>
@@ -4700,17 +4889,17 @@
       </c>
       <c r="Y43" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VIII-M-A FRUTICULTURA </v>
+        <v>AG_VIII-M-A FRUTICULTURA</v>
       </c>
       <c r="Z43" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S43,"' target='_blank'&gt;&lt;img src='",AC43,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Hl9vlkN6Tcc0W5Gv3ek4CK' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA43" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="AB43" t="s">
         <v>334</v>
-      </c>
-      <c r="AB43" t="s">
-        <v>335</v>
       </c>
       <c r="AC43" s="8" t="s">
         <v>234</v>
@@ -4771,17 +4960,17 @@
       </c>
       <c r="Y44" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">AG_VIII-T-B FRUTICULTURA </v>
+        <v>AG_VIII-T-B FRUTICULTURA</v>
       </c>
       <c r="Z44" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S44,"' target='_blank'&gt;&lt;img src='",AC44,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Hkdo8BCbdYF0r7lK0zDcx0' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA44" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="AB44" t="s">
         <v>336</v>
-      </c>
-      <c r="AB44" t="s">
-        <v>337</v>
       </c>
       <c r="AC44" s="8" t="s">
         <v>234</v>
@@ -4845,14 +5034,14 @@
         <v>AG_VIII-M-A ENTOMOLOGÍA A</v>
       </c>
       <c r="Z45" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S45,"' target='_blank'&gt;&lt;img src='",AC45,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/BSjyRn0v7Hd0RZAwKDelHI' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA45" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB45" t="s">
         <v>338</v>
-      </c>
-      <c r="AB45" t="s">
-        <v>339</v>
       </c>
       <c r="AC45" s="8" t="s">
         <v>234</v>
@@ -4916,14 +5105,14 @@
         <v>AG_VIII-T-B ENTOMOLOGÍA A</v>
       </c>
       <c r="Z46" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S46,"' target='_blank'&gt;&lt;img src='",AC46,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/K1mkJtwQJheK0xmAS0WQ95' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA46" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB46" t="s">
         <v>340</v>
-      </c>
-      <c r="AB46" t="s">
-        <v>341</v>
       </c>
       <c r="AC46" s="8" t="s">
         <v>234</v>
@@ -4987,14 +5176,14 @@
         <v>AG_VIII-M-A METODOLOGÍA D</v>
       </c>
       <c r="Z47" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S47,"' target='_blank'&gt;&lt;img src='",AC47,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/DHQUOVl6iAN93UzdOo3ipP' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA47" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AB47" t="s">
         <v>342</v>
-      </c>
-      <c r="AB47" t="s">
-        <v>343</v>
       </c>
       <c r="AC47" s="8" t="s">
         <v>234</v>
@@ -5058,14 +5247,14 @@
         <v>AG_VIII-T-B METODOLOGÍA D</v>
       </c>
       <c r="Z48" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S48,"' target='_blank'&gt;&lt;img src='",AC48,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EuhBbZ2mUVELCseDu0pCgA' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA48" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="AB48" t="s">
         <v>344</v>
-      </c>
-      <c r="AB48" t="s">
-        <v>345</v>
       </c>
       <c r="AC48" s="8" t="s">
         <v>234</v>
@@ -5129,14 +5318,14 @@
         <v>AG_VIII-M-A PRODUCCIÓN DE</v>
       </c>
       <c r="Z49" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S49,"' target='_blank'&gt;&lt;img src='",AC49,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Gs9BoN9Rtu01X277ysceDD' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA49" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB49" t="s">
         <v>346</v>
-      </c>
-      <c r="AB49" t="s">
-        <v>347</v>
       </c>
       <c r="AC49" s="8" t="s">
         <v>234</v>
@@ -5200,14 +5389,14 @@
         <v>AG_VIII-T-B PRODUCCIÓN DE</v>
       </c>
       <c r="Z50" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S50,"' target='_blank'&gt;&lt;img src='",AC50,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EXaZtVMPIOxAZeyWFXg21A' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA50" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="AB50" t="s">
         <v>348</v>
-      </c>
-      <c r="AB50" t="s">
-        <v>349</v>
       </c>
       <c r="AC50" s="8" t="s">
         <v>234</v>
@@ -5271,14 +5460,14 @@
         <v>AG_X-M-A FORMULACIÓN Y EV</v>
       </c>
       <c r="Z51" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S51,"' target='_blank'&gt;&lt;img src='",AC51,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FNJFXk5PFtyK2OP4LPVBP8' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA51" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB51" t="s">
         <v>350</v>
-      </c>
-      <c r="AB51" t="s">
-        <v>351</v>
       </c>
       <c r="AC51" s="8" t="s">
         <v>234</v>
@@ -5342,14 +5531,14 @@
         <v>AG_X-T-B FORMULACIÓN Y EV</v>
       </c>
       <c r="Z52" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S52,"' target='_blank'&gt;&lt;img src='",AC52,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Cc6suyo0sVg7rzH29f1xNY' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA52" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB52" t="s">
         <v>352</v>
-      </c>
-      <c r="AB52" t="s">
-        <v>353</v>
       </c>
       <c r="AC52" s="8" t="s">
         <v>234</v>
@@ -5413,14 +5602,14 @@
         <v>AG_X-M-A EXTENSIÓN AGRARI</v>
       </c>
       <c r="Z53" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S53,"' target='_blank'&gt;&lt;img src='",AC53,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/EC78puZGT5G9RVgwd6G4Y3' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA53" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="AB53" t="s">
         <v>354</v>
-      </c>
-      <c r="AB53" t="s">
-        <v>355</v>
       </c>
       <c r="AC53" s="8" t="s">
         <v>234</v>
@@ -5484,14 +5673,14 @@
         <v>AG_X-T-B EXTENSIÓN AGRARI</v>
       </c>
       <c r="Z54" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S54,"' target='_blank'&gt;&lt;img src='",AC54,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/FEAScn7L5txEH8ePcre5Rx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA54" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB54" t="s">
         <v>356</v>
-      </c>
-      <c r="AB54" t="s">
-        <v>357</v>
       </c>
       <c r="AC54" s="8" t="s">
         <v>234</v>
@@ -5555,14 +5744,14 @@
         <v>AG_X-M-A MANEJO INTEGRADO</v>
       </c>
       <c r="Z55" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S55,"' target='_blank'&gt;&lt;img src='",AC55,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J8mVfTRHEoC1V8nyMEIk56' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA55" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB55" t="s">
         <v>358</v>
-      </c>
-      <c r="AB55" t="s">
-        <v>359</v>
       </c>
       <c r="AC55" s="8" t="s">
         <v>234</v>
@@ -5626,14 +5815,14 @@
         <v>AG_X-T-B MANEJO INTEGRADO</v>
       </c>
       <c r="Z56" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S56,"' target='_blank'&gt;&lt;img src='",AC56,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/GOURuZSLUyr3hVVuHRLymg' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA56" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB56" t="s">
         <v>360</v>
-      </c>
-      <c r="AB56" t="s">
-        <v>361</v>
       </c>
       <c r="AC56" s="8" t="s">
         <v>234</v>
@@ -5697,14 +5886,14 @@
         <v>AG_X-M-A SEMINARIO DE TES</v>
       </c>
       <c r="Z57" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S57,"' target='_blank'&gt;&lt;img src='",AC57,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/CXwOXFiDI10CwNgEz0axhc' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA57" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="AB57" t="s">
         <v>362</v>
-      </c>
-      <c r="AB57" t="s">
-        <v>363</v>
       </c>
       <c r="AC57" s="8" t="s">
         <v>234</v>
@@ -5768,14 +5957,14 @@
         <v>AG_X-T-B SEMINARIO DE TES</v>
       </c>
       <c r="Z58" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S58,"' target='_blank'&gt;&lt;img src='",AC58,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/J1wt04kGjN89WKPhT7XmLf' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA58" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="AB58" t="s">
         <v>364</v>
-      </c>
-      <c r="AB58" t="s">
-        <v>365</v>
       </c>
       <c r="AC58" s="8" t="s">
         <v>234</v>
@@ -5839,14 +6028,14 @@
         <v>AG_X-M-A NUTRICIÓN Y ALIM</v>
       </c>
       <c r="Z59" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S59,"' target='_blank'&gt;&lt;img src='",AC59,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IqffUMSFMCpFLYeOhWsySp' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA59" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="AB59" t="s">
         <v>366</v>
-      </c>
-      <c r="AB59" t="s">
-        <v>367</v>
       </c>
       <c r="AC59" s="8" t="s">
         <v>234</v>
@@ -5910,14 +6099,14 @@
         <v>AG_X-T-B NUTRICIÓN Y ALIM</v>
       </c>
       <c r="Z60" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S60,"' target='_blank'&gt;&lt;img src='",AC60,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IPQiyFFNNjpB3Fkgg3b0ZJ' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA60" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="AB60" t="s">
         <v>368</v>
-      </c>
-      <c r="AB60" t="s">
-        <v>369</v>
       </c>
       <c r="AC60" s="8" t="s">
         <v>234</v>
@@ -5981,14 +6170,14 @@
         <v>AG_X-M-A CONTROL BIOLÓGIC</v>
       </c>
       <c r="Z61" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S61,"' target='_blank'&gt;&lt;img src='",AC61,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Ev0qZ2cGlfxAY7oKZvU0Wb' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA61" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AB61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AC61" s="8" t="s">
         <v>234</v>
@@ -6052,14 +6241,14 @@
         <v>AG_X-T-B CONTROL BIOLÓGIC</v>
       </c>
       <c r="Z62" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S62,"' target='_blank'&gt;&lt;img src='",AC62,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Kwo6hH8eEQ9CBJzEcjLmbX' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA62" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="AB62" t="s">
         <v>371</v>
-      </c>
-      <c r="AB62" t="s">
-        <v>372</v>
       </c>
       <c r="AC62" s="8" t="s">
         <v>234</v>
@@ -6123,14 +6312,14 @@
         <v>AG_X-M-A AGRICULTURA ORGÁ</v>
       </c>
       <c r="Z63" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S63,"' target='_blank'&gt;&lt;img src='",AC63,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/JkjOSwZ5t5d7mMPwQo9bha' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA63" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="AB63" t="s">
         <v>373</v>
-      </c>
-      <c r="AB63" t="s">
-        <v>374</v>
       </c>
       <c r="AC63" s="8" t="s">
         <v>234</v>
@@ -6191,14 +6380,14 @@
         <v>AG_X-T-B AGRICULTURA ORGÁ</v>
       </c>
       <c r="Z64" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S64,"' target='_blank'&gt;&lt;img src='",AC64,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/KFYFa47lVAB0TvkCAxJOfx' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA64" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB64" t="s">
         <v>375</v>
-      </c>
-      <c r="AB64" t="s">
-        <v>376</v>
       </c>
       <c r="AC64" s="8" t="s">
         <v>234</v>
@@ -6215,10 +6404,10 @@
         <v>9</v>
       </c>
       <c r="D65" t="s">
+        <v>235</v>
+      </c>
+      <c r="E65" t="s">
         <v>236</v>
-      </c>
-      <c r="E65" t="s">
-        <v>237</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
@@ -6230,43 +6419,43 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="T65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U65" t="str">
         <f t="shared" si="4"/>
         <v>1150</v>
       </c>
       <c r="V65" t="str">
-        <f t="shared" ref="V65:V66" si="9">MID(D65,1,10)</f>
+        <f t="shared" ref="V65:V66" si="10">MID(D65,1,10)</f>
         <v>AG36 - 566</v>
       </c>
       <c r="W65" t="str">
-        <f t="shared" ref="W65:W66" si="10">TRIM(MID(D65,14,222))</f>
+        <f t="shared" ref="W65:W66" si="11">TRIM(MID(D65,14,222))</f>
         <v>MATEMÁTICA II - 2850</v>
       </c>
       <c r="X65" t="str">
-        <f t="shared" ref="X65:X66" si="11">CONCATENATE(B65,"_",E65,"-",F65,"-",G65," ",W65)</f>
+        <f t="shared" ref="X65:X66" si="12">CONCATENATE(B65,"_",E65,"-",F65,"-",G65," ",W65)</f>
         <v>AG_III-M-A MATEMÁTICA II - 2850</v>
       </c>
       <c r="Y65" t="str">
-        <f t="shared" ref="Y65:Y66" si="12">MID(X65,1,25)</f>
-        <v xml:space="preserve">AG_III-M-A MATEMÁTICA II </v>
+        <f t="shared" si="8"/>
+        <v>AG_III-M-A MATEMÁTICA II</v>
       </c>
       <c r="Z65" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S65,"' target='_blank'&gt;&lt;img src='",AC65,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/H8JTCbxGrMAEgkdI38jH6F' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA65" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="AB65" t="s">
         <v>377</v>
-      </c>
-      <c r="AB65" t="s">
-        <v>378</v>
       </c>
       <c r="AC65" s="8" t="s">
         <v>234</v>
@@ -6283,10 +6472,10 @@
         <v>9</v>
       </c>
       <c r="D66" t="s">
+        <v>238</v>
+      </c>
+      <c r="E66" t="s">
         <v>239</v>
-      </c>
-      <c r="E66" t="s">
-        <v>240</v>
       </c>
       <c r="F66" t="s">
         <v>9</v>
@@ -6298,43 +6487,43 @@
         <v>34</v>
       </c>
       <c r="I66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S66" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T66" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U66" t="str">
         <f t="shared" si="4"/>
         <v>1149</v>
       </c>
       <c r="V66" t="str">
+        <f t="shared" si="10"/>
+        <v>CB.1 - 677</v>
+      </c>
+      <c r="W66" t="str">
+        <f t="shared" si="11"/>
+        <v>MATEMÁTICA BÁSICA - 2849</v>
+      </c>
+      <c r="X66" t="str">
+        <f t="shared" si="12"/>
+        <v>AG_I-M-A MATEMÁTICA BÁSICA - 2849</v>
+      </c>
+      <c r="Y66" t="str">
+        <f t="shared" si="8"/>
+        <v>AG_I-M-A MATEMÁTICA BÁSIC</v>
+      </c>
+      <c r="Z66" t="str">
         <f t="shared" si="9"/>
-        <v>CB.1 - 677</v>
-      </c>
-      <c r="W66" t="str">
-        <f t="shared" si="10"/>
-        <v>MATEMÁTICA BÁSICA - 2849</v>
-      </c>
-      <c r="X66" t="str">
-        <f t="shared" si="11"/>
-        <v>AG_I-M-A MATEMÁTICA BÁSICA - 2849</v>
-      </c>
-      <c r="Y66" t="str">
-        <f t="shared" si="12"/>
-        <v>AG_I-M-A MATEMÁTICA BÁSIC</v>
-      </c>
-      <c r="Z66" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S66,"' target='_blank'&gt;&lt;img src='",AC66,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/C9Ncjfw6CxfDZfS5Z4ngkh' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA66" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="AB66" t="s">
         <v>379</v>
-      </c>
-      <c r="AB66" t="s">
-        <v>380</v>
       </c>
       <c r="AC66" s="8" t="s">
         <v>234</v>
@@ -6348,7 +6537,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E67" t="s">
         <v>18</v>
@@ -6360,10 +6549,10 @@
         <v>11</v>
       </c>
       <c r="I67" t="s">
+        <v>244</v>
+      </c>
+      <c r="T67" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="T67" s="9" t="s">
-        <v>246</v>
       </c>
       <c r="U67" t="str">
         <f t="shared" ref="U67" si="13">MID(T67,45,4)</f>
@@ -6382,18 +6571,18 @@
         <v>AG_V-T-B EDAFOLOGIA - 2756</v>
       </c>
       <c r="Y67" t="str">
-        <f t="shared" ref="Y67" si="17">MID(X67,1,25)</f>
+        <f t="shared" ref="Y67" si="17">TRIM(MID(X67,1,25))</f>
         <v>AG_V-T-B EDAFOLOGIA - 275</v>
       </c>
       <c r="Z67" t="str">
-        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S67,"' target='_blank'&gt;&lt;img src='",AC67,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <f t="shared" si="9"/>
         <v>&lt;p&gt;&lt;a href='' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
       <c r="AA67" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="AB67" t="s">
         <v>381</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>382</v>
       </c>
       <c r="AC67" s="8" t="s">
         <v>234</v>
@@ -6478,20 +6667,336 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956E4737-6198-4B8E-ADF8-148D6104AE44}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="B1"/>
+  <dimension ref="B1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>235</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>